<commit_message>
complete code for report khach hang
</commit_message>
<xml_diff>
--- a/notion_data/LUY_KE_NGAY_CAN_THO.xlsx
+++ b/notion_data/LUY_KE_NGAY_CAN_THO.xlsx
@@ -688,7 +688,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2024-07-04T08:33:00.000Z</t>
+          <t>2024-07-04T09:36:00.000Z</t>
         </is>
       </c>
       <c r="E2" t="inlineStr"/>
@@ -887,7 +887,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2024-07-04T08:33:00.000Z</t>
+          <t>2024-07-04T09:36:00.000Z</t>
         </is>
       </c>
       <c r="E3" t="inlineStr"/>
@@ -1086,7 +1086,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>2024-07-04T08:33:00.000Z</t>
+          <t>2024-07-04T09:36:00.000Z</t>
         </is>
       </c>
       <c r="E4" t="inlineStr"/>
@@ -1285,7 +1285,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2024-07-04T08:33:00.000Z</t>
+          <t>2024-07-04T09:36:00.000Z</t>
         </is>
       </c>
       <c r="E5" t="inlineStr"/>
@@ -1484,7 +1484,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2024-07-04T08:33:00.000Z</t>
+          <t>2024-07-04T09:36:00.000Z</t>
         </is>
       </c>
       <c r="E6" t="inlineStr"/>
@@ -1683,7 +1683,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>2024-07-04T08:33:00.000Z</t>
+          <t>2024-07-04T09:36:00.000Z</t>
         </is>
       </c>
       <c r="E7" t="inlineStr"/>
@@ -1882,7 +1882,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>2024-07-04T08:33:00.000Z</t>
+          <t>2024-07-04T09:36:00.000Z</t>
         </is>
       </c>
       <c r="E8" t="inlineStr"/>
@@ -2081,7 +2081,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>2024-07-04T08:33:00.000Z</t>
+          <t>2024-07-04T09:36:00.000Z</t>
         </is>
       </c>
       <c r="E9" t="inlineStr"/>
@@ -2280,7 +2280,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>2024-07-04T08:33:00.000Z</t>
+          <t>2024-07-04T09:36:00.000Z</t>
         </is>
       </c>
       <c r="E10" t="inlineStr"/>
@@ -2479,7 +2479,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>2024-07-04T08:33:00.000Z</t>
+          <t>2024-07-04T09:36:00.000Z</t>
         </is>
       </c>
       <c r="E11" t="inlineStr"/>
@@ -2678,7 +2678,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>2024-07-04T08:33:00.000Z</t>
+          <t>2024-07-04T09:36:00.000Z</t>
         </is>
       </c>
       <c r="E12" t="inlineStr"/>
@@ -2877,7 +2877,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>2024-07-04T08:33:00.000Z</t>
+          <t>2024-07-04T09:36:00.000Z</t>
         </is>
       </c>
       <c r="E13" t="inlineStr"/>
@@ -3076,7 +3076,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>2024-07-04T08:33:00.000Z</t>
+          <t>2024-07-04T09:33:00.000Z</t>
         </is>
       </c>
       <c r="E14" t="inlineStr"/>
@@ -3275,7 +3275,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>2024-07-04T08:33:00.000Z</t>
+          <t>2024-07-04T09:33:00.000Z</t>
         </is>
       </c>
       <c r="E15" t="inlineStr"/>
@@ -3474,7 +3474,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>2024-07-04T08:33:00.000Z</t>
+          <t>2024-07-04T09:33:00.000Z</t>
         </is>
       </c>
       <c r="E16" t="inlineStr"/>
@@ -3673,7 +3673,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>2024-07-04T08:33:00.000Z</t>
+          <t>2024-07-04T09:33:00.000Z</t>
         </is>
       </c>
       <c r="E17" t="inlineStr"/>
@@ -3872,7 +3872,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>2024-07-04T08:33:00.000Z</t>
+          <t>2024-07-04T09:33:00.000Z</t>
         </is>
       </c>
       <c r="E18" t="inlineStr"/>
@@ -4071,7 +4071,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>2024-07-04T08:33:00.000Z</t>
+          <t>2024-07-04T09:33:00.000Z</t>
         </is>
       </c>
       <c r="E19" t="inlineStr"/>
@@ -4270,7 +4270,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>2024-07-04T08:33:00.000Z</t>
+          <t>2024-07-04T09:33:00.000Z</t>
         </is>
       </c>
       <c r="E20" t="inlineStr"/>
@@ -4469,7 +4469,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>2024-07-04T08:33:00.000Z</t>
+          <t>2024-07-04T09:33:00.000Z</t>
         </is>
       </c>
       <c r="E21" t="inlineStr"/>
@@ -4668,7 +4668,7 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>2024-07-04T08:33:00.000Z</t>
+          <t>2024-07-04T09:33:00.000Z</t>
         </is>
       </c>
       <c r="E22" t="inlineStr"/>
@@ -4867,7 +4867,7 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>2024-07-04T08:33:00.000Z</t>
+          <t>2024-07-04T09:33:00.000Z</t>
         </is>
       </c>
       <c r="E23" t="inlineStr"/>
@@ -5066,7 +5066,7 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>2024-07-04T08:33:00.000Z</t>
+          <t>2024-07-04T09:33:00.000Z</t>
         </is>
       </c>
       <c r="E24" t="inlineStr"/>
@@ -5265,7 +5265,7 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>2024-07-04T08:33:00.000Z</t>
+          <t>2024-07-04T09:33:00.000Z</t>
         </is>
       </c>
       <c r="E25" t="inlineStr"/>
@@ -5464,7 +5464,7 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>2024-07-04T08:33:00.000Z</t>
+          <t>2024-07-04T09:33:00.000Z</t>
         </is>
       </c>
       <c r="E26" t="inlineStr"/>
@@ -5663,7 +5663,7 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>2024-07-04T08:33:00.000Z</t>
+          <t>2024-07-04T09:33:00.000Z</t>
         </is>
       </c>
       <c r="E27" t="inlineStr"/>
@@ -5862,7 +5862,7 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>2024-07-04T08:33:00.000Z</t>
+          <t>2024-07-04T09:33:00.000Z</t>
         </is>
       </c>
       <c r="E28" t="inlineStr"/>
@@ -6061,7 +6061,7 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>2024-07-04T08:33:00.000Z</t>
+          <t>2024-07-04T09:33:00.000Z</t>
         </is>
       </c>
       <c r="E29" t="inlineStr"/>
@@ -6260,7 +6260,7 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>2024-07-04T08:33:00.000Z</t>
+          <t>2024-07-04T09:33:00.000Z</t>
         </is>
       </c>
       <c r="E30" t="inlineStr"/>
@@ -6459,7 +6459,7 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>2024-07-04T08:33:00.000Z</t>
+          <t>2024-07-04T09:34:00.000Z</t>
         </is>
       </c>
       <c r="E31" t="inlineStr"/>
@@ -6658,7 +6658,7 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>2024-07-04T08:33:00.000Z</t>
+          <t>2024-07-04T09:34:00.000Z</t>
         </is>
       </c>
       <c r="E32" t="inlineStr"/>
@@ -6857,7 +6857,7 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>2024-07-04T08:33:00.000Z</t>
+          <t>2024-07-04T09:34:00.000Z</t>
         </is>
       </c>
       <c r="E33" t="inlineStr"/>
@@ -7056,7 +7056,7 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>2024-07-04T08:33:00.000Z</t>
+          <t>2024-07-04T09:34:00.000Z</t>
         </is>
       </c>
       <c r="E34" t="inlineStr"/>
@@ -7255,7 +7255,7 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>2024-07-04T08:33:00.000Z</t>
+          <t>2024-07-04T09:34:00.000Z</t>
         </is>
       </c>
       <c r="E35" t="inlineStr"/>
@@ -7454,7 +7454,7 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>2024-07-04T08:33:00.000Z</t>
+          <t>2024-07-04T09:34:00.000Z</t>
         </is>
       </c>
       <c r="E36" t="inlineStr"/>
@@ -7653,7 +7653,7 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>2024-07-04T08:33:00.000Z</t>
+          <t>2024-07-04T09:34:00.000Z</t>
         </is>
       </c>
       <c r="E37" t="inlineStr"/>
@@ -7852,7 +7852,7 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>2024-07-04T08:33:00.000Z</t>
+          <t>2024-07-04T09:34:00.000Z</t>
         </is>
       </c>
       <c r="E38" t="inlineStr"/>
@@ -8051,7 +8051,7 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>2024-07-04T08:34:00.000Z</t>
+          <t>2024-07-04T09:34:00.000Z</t>
         </is>
       </c>
       <c r="E39" t="inlineStr"/>
@@ -8250,7 +8250,7 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>2024-07-04T08:34:00.000Z</t>
+          <t>2024-07-04T09:34:00.000Z</t>
         </is>
       </c>
       <c r="E40" t="inlineStr"/>
@@ -8449,7 +8449,7 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>2024-07-04T08:34:00.000Z</t>
+          <t>2024-07-04T09:34:00.000Z</t>
         </is>
       </c>
       <c r="E41" t="inlineStr"/>
@@ -8648,7 +8648,7 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>2024-07-04T08:34:00.000Z</t>
+          <t>2024-07-04T09:34:00.000Z</t>
         </is>
       </c>
       <c r="E42" t="inlineStr"/>
@@ -8847,7 +8847,7 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>2024-07-04T08:34:00.000Z</t>
+          <t>2024-07-04T09:34:00.000Z</t>
         </is>
       </c>
       <c r="E43" t="inlineStr"/>
@@ -9046,7 +9046,7 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>2024-07-04T08:34:00.000Z</t>
+          <t>2024-07-04T09:34:00.000Z</t>
         </is>
       </c>
       <c r="E44" t="inlineStr"/>
@@ -9245,7 +9245,7 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>2024-07-04T08:34:00.000Z</t>
+          <t>2024-07-04T09:34:00.000Z</t>
         </is>
       </c>
       <c r="E45" t="inlineStr"/>
@@ -9444,7 +9444,7 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>2024-07-04T08:34:00.000Z</t>
+          <t>2024-07-04T09:34:00.000Z</t>
         </is>
       </c>
       <c r="E46" t="inlineStr"/>
@@ -9643,7 +9643,7 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>2024-07-04T08:34:00.000Z</t>
+          <t>2024-07-04T09:34:00.000Z</t>
         </is>
       </c>
       <c r="E47" t="inlineStr"/>
@@ -9842,7 +9842,7 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>2024-07-04T08:34:00.000Z</t>
+          <t>2024-07-04T09:34:00.000Z</t>
         </is>
       </c>
       <c r="E48" t="inlineStr"/>
@@ -10041,7 +10041,7 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>2024-07-04T08:34:00.000Z</t>
+          <t>2024-07-04T09:34:00.000Z</t>
         </is>
       </c>
       <c r="E49" t="inlineStr"/>
@@ -10240,7 +10240,7 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>2024-07-04T08:34:00.000Z</t>
+          <t>2024-07-04T09:34:00.000Z</t>
         </is>
       </c>
       <c r="E50" t="inlineStr"/>
@@ -10439,7 +10439,7 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>2024-07-04T08:34:00.000Z</t>
+          <t>2024-07-04T09:34:00.000Z</t>
         </is>
       </c>
       <c r="E51" t="inlineStr"/>
@@ -10638,7 +10638,7 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>2024-07-04T08:34:00.000Z</t>
+          <t>2024-07-04T09:34:00.000Z</t>
         </is>
       </c>
       <c r="E52" t="inlineStr"/>
@@ -10837,7 +10837,7 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>2024-07-04T08:34:00.000Z</t>
+          <t>2024-07-04T09:34:00.000Z</t>
         </is>
       </c>
       <c r="E53" t="inlineStr"/>
@@ -11036,7 +11036,7 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>2024-07-04T08:34:00.000Z</t>
+          <t>2024-07-04T09:34:00.000Z</t>
         </is>
       </c>
       <c r="E54" t="inlineStr"/>
@@ -11235,7 +11235,7 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>2024-07-04T08:34:00.000Z</t>
+          <t>2024-07-04T09:34:00.000Z</t>
         </is>
       </c>
       <c r="E55" t="inlineStr"/>
@@ -11434,7 +11434,7 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>2024-07-04T08:34:00.000Z</t>
+          <t>2024-07-04T09:34:00.000Z</t>
         </is>
       </c>
       <c r="E56" t="inlineStr"/>
@@ -11633,7 +11633,7 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>2024-07-04T08:34:00.000Z</t>
+          <t>2024-07-04T09:34:00.000Z</t>
         </is>
       </c>
       <c r="E57" t="inlineStr"/>
@@ -11832,7 +11832,7 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>2024-07-04T08:34:00.000Z</t>
+          <t>2024-07-04T09:34:00.000Z</t>
         </is>
       </c>
       <c r="E58" t="inlineStr"/>
@@ -12031,7 +12031,7 @@
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>2024-07-04T08:34:00.000Z</t>
+          <t>2024-07-04T09:34:00.000Z</t>
         </is>
       </c>
       <c r="E59" t="inlineStr"/>
@@ -12230,7 +12230,7 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>2024-07-04T08:34:00.000Z</t>
+          <t>2024-07-04T09:34:00.000Z</t>
         </is>
       </c>
       <c r="E60" t="inlineStr"/>
@@ -12429,7 +12429,7 @@
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>2024-07-04T08:34:00.000Z</t>
+          <t>2024-07-04T09:34:00.000Z</t>
         </is>
       </c>
       <c r="E61" t="inlineStr"/>
@@ -12628,7 +12628,7 @@
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>2024-07-04T08:34:00.000Z</t>
+          <t>2024-07-04T09:34:00.000Z</t>
         </is>
       </c>
       <c r="E62" t="inlineStr"/>
@@ -12827,7 +12827,7 @@
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>2024-07-04T08:34:00.000Z</t>
+          <t>2024-07-04T09:34:00.000Z</t>
         </is>
       </c>
       <c r="E63" t="inlineStr"/>
@@ -13026,7 +13026,7 @@
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>2024-07-04T08:34:00.000Z</t>
+          <t>2024-07-04T09:34:00.000Z</t>
         </is>
       </c>
       <c r="E64" t="inlineStr"/>
@@ -13225,7 +13225,7 @@
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>2024-07-04T08:34:00.000Z</t>
+          <t>2024-07-04T09:34:00.000Z</t>
         </is>
       </c>
       <c r="E65" t="inlineStr"/>
@@ -13424,7 +13424,7 @@
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>2024-07-04T08:34:00.000Z</t>
+          <t>2024-07-04T09:34:00.000Z</t>
         </is>
       </c>
       <c r="E66" t="inlineStr"/>
@@ -13623,7 +13623,7 @@
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>2024-07-04T08:34:00.000Z</t>
+          <t>2024-07-04T09:34:00.000Z</t>
         </is>
       </c>
       <c r="E67" t="inlineStr"/>
@@ -13822,7 +13822,7 @@
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>2024-07-04T08:34:00.000Z</t>
+          <t>2024-07-04T09:34:00.000Z</t>
         </is>
       </c>
       <c r="E68" t="inlineStr"/>
@@ -14021,7 +14021,7 @@
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>2024-07-04T08:34:00.000Z</t>
+          <t>2024-07-04T09:34:00.000Z</t>
         </is>
       </c>
       <c r="E69" t="inlineStr"/>
@@ -14220,7 +14220,7 @@
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>2024-07-04T08:34:00.000Z</t>
+          <t>2024-07-04T09:34:00.000Z</t>
         </is>
       </c>
       <c r="E70" t="inlineStr"/>
@@ -14419,7 +14419,7 @@
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>2024-07-04T08:34:00.000Z</t>
+          <t>2024-07-04T09:34:00.000Z</t>
         </is>
       </c>
       <c r="E71" t="inlineStr"/>
@@ -14618,7 +14618,7 @@
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>2024-07-04T08:34:00.000Z</t>
+          <t>2024-07-04T09:34:00.000Z</t>
         </is>
       </c>
       <c r="E72" t="inlineStr"/>
@@ -14817,7 +14817,7 @@
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>2024-07-04T08:34:00.000Z</t>
+          <t>2024-07-04T09:34:00.000Z</t>
         </is>
       </c>
       <c r="E73" t="inlineStr"/>
@@ -15016,7 +15016,7 @@
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>2024-07-04T08:34:00.000Z</t>
+          <t>2024-07-04T09:34:00.000Z</t>
         </is>
       </c>
       <c r="E74" t="inlineStr"/>
@@ -15215,7 +15215,7 @@
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>2024-07-04T08:34:00.000Z</t>
+          <t>2024-07-04T09:34:00.000Z</t>
         </is>
       </c>
       <c r="E75" t="inlineStr"/>
@@ -15414,7 +15414,7 @@
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>2024-07-04T08:34:00.000Z</t>
+          <t>2024-07-04T09:34:00.000Z</t>
         </is>
       </c>
       <c r="E76" t="inlineStr"/>
@@ -15613,7 +15613,7 @@
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>2024-07-04T08:34:00.000Z</t>
+          <t>2024-07-04T09:35:00.000Z</t>
         </is>
       </c>
       <c r="E77" t="inlineStr"/>
@@ -15812,7 +15812,7 @@
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>2024-07-04T08:34:00.000Z</t>
+          <t>2024-07-04T09:35:00.000Z</t>
         </is>
       </c>
       <c r="E78" t="inlineStr"/>
@@ -16011,7 +16011,7 @@
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>2024-07-04T08:34:00.000Z</t>
+          <t>2024-07-04T09:35:00.000Z</t>
         </is>
       </c>
       <c r="E79" t="inlineStr"/>
@@ -16210,7 +16210,7 @@
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>2024-07-04T08:34:00.000Z</t>
+          <t>2024-07-04T09:35:00.000Z</t>
         </is>
       </c>
       <c r="E80" t="inlineStr"/>
@@ -16409,7 +16409,7 @@
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>2024-07-04T08:34:00.000Z</t>
+          <t>2024-07-04T09:35:00.000Z</t>
         </is>
       </c>
       <c r="E81" t="inlineStr"/>
@@ -16608,7 +16608,7 @@
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>2024-07-04T08:34:00.000Z</t>
+          <t>2024-07-04T09:35:00.000Z</t>
         </is>
       </c>
       <c r="E82" t="inlineStr"/>
@@ -16807,7 +16807,7 @@
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>2024-07-04T08:34:00.000Z</t>
+          <t>2024-07-04T09:35:00.000Z</t>
         </is>
       </c>
       <c r="E83" t="inlineStr"/>
@@ -17006,7 +17006,7 @@
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>2024-07-04T08:34:00.000Z</t>
+          <t>2024-07-04T09:35:00.000Z</t>
         </is>
       </c>
       <c r="E84" t="inlineStr"/>
@@ -17205,7 +17205,7 @@
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>2024-07-04T08:35:00.000Z</t>
+          <t>2024-07-04T09:35:00.000Z</t>
         </is>
       </c>
       <c r="E85" t="inlineStr"/>
@@ -17404,7 +17404,7 @@
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>2024-07-04T08:35:00.000Z</t>
+          <t>2024-07-04T09:35:00.000Z</t>
         </is>
       </c>
       <c r="E86" t="inlineStr"/>
@@ -17603,7 +17603,7 @@
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>2024-07-04T08:35:00.000Z</t>
+          <t>2024-07-04T09:35:00.000Z</t>
         </is>
       </c>
       <c r="E87" t="inlineStr"/>
@@ -17802,7 +17802,7 @@
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>2024-07-04T08:35:00.000Z</t>
+          <t>2024-07-04T09:35:00.000Z</t>
         </is>
       </c>
       <c r="E88" t="inlineStr"/>
@@ -18001,7 +18001,7 @@
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>2024-07-04T08:35:00.000Z</t>
+          <t>2024-07-04T09:35:00.000Z</t>
         </is>
       </c>
       <c r="E89" t="inlineStr"/>
@@ -18200,7 +18200,7 @@
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>2024-07-04T08:35:00.000Z</t>
+          <t>2024-07-04T09:35:00.000Z</t>
         </is>
       </c>
       <c r="E90" t="inlineStr"/>
@@ -18399,7 +18399,7 @@
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>2024-07-04T08:35:00.000Z</t>
+          <t>2024-07-04T09:35:00.000Z</t>
         </is>
       </c>
       <c r="E91" t="inlineStr"/>
@@ -18598,7 +18598,7 @@
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>2024-07-04T08:35:00.000Z</t>
+          <t>2024-07-04T09:35:00.000Z</t>
         </is>
       </c>
       <c r="E92" t="inlineStr"/>
@@ -18797,7 +18797,7 @@
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>2024-07-04T08:35:00.000Z</t>
+          <t>2024-07-04T09:35:00.000Z</t>
         </is>
       </c>
       <c r="E93" t="inlineStr"/>
@@ -18996,7 +18996,7 @@
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>2024-07-04T08:35:00.000Z</t>
+          <t>2024-07-04T09:35:00.000Z</t>
         </is>
       </c>
       <c r="E94" t="inlineStr"/>
@@ -19195,7 +19195,7 @@
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>2024-07-04T08:35:00.000Z</t>
+          <t>2024-07-04T09:35:00.000Z</t>
         </is>
       </c>
       <c r="E95" t="inlineStr"/>
@@ -19394,7 +19394,7 @@
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>2024-07-04T08:35:00.000Z</t>
+          <t>2024-07-04T09:35:00.000Z</t>
         </is>
       </c>
       <c r="E96" t="inlineStr"/>
@@ -19593,7 +19593,7 @@
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>2024-07-04T08:35:00.000Z</t>
+          <t>2024-07-04T09:35:00.000Z</t>
         </is>
       </c>
       <c r="E97" t="inlineStr"/>
@@ -19792,7 +19792,7 @@
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>2024-07-04T08:35:00.000Z</t>
+          <t>2024-07-04T09:35:00.000Z</t>
         </is>
       </c>
       <c r="E98" t="inlineStr"/>
@@ -19991,7 +19991,7 @@
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>2024-07-04T08:35:00.000Z</t>
+          <t>2024-07-04T09:35:00.000Z</t>
         </is>
       </c>
       <c r="E99" t="inlineStr"/>
@@ -20190,7 +20190,7 @@
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>2024-07-04T08:35:00.000Z</t>
+          <t>2024-07-04T09:35:00.000Z</t>
         </is>
       </c>
       <c r="E100" t="inlineStr"/>
@@ -20389,7 +20389,7 @@
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>2024-07-04T08:35:00.000Z</t>
+          <t>2024-07-04T09:35:00.000Z</t>
         </is>
       </c>
       <c r="E101" t="inlineStr"/>
@@ -20588,7 +20588,7 @@
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>2024-07-04T08:35:00.000Z</t>
+          <t>2024-07-04T09:35:00.000Z</t>
         </is>
       </c>
       <c r="E102" t="inlineStr"/>
@@ -20787,7 +20787,7 @@
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>2024-07-04T08:35:00.000Z</t>
+          <t>2024-07-04T09:35:00.000Z</t>
         </is>
       </c>
       <c r="E103" t="inlineStr"/>
@@ -20986,7 +20986,7 @@
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>2024-07-04T08:35:00.000Z</t>
+          <t>2024-07-04T09:35:00.000Z</t>
         </is>
       </c>
       <c r="E104" t="inlineStr"/>
@@ -21185,7 +21185,7 @@
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>2024-07-04T08:35:00.000Z</t>
+          <t>2024-07-04T09:35:00.000Z</t>
         </is>
       </c>
       <c r="E105" t="inlineStr"/>
@@ -21384,7 +21384,7 @@
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>2024-07-04T08:35:00.000Z</t>
+          <t>2024-07-04T09:35:00.000Z</t>
         </is>
       </c>
       <c r="E106" t="inlineStr"/>
@@ -21583,7 +21583,7 @@
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>2024-07-04T08:35:00.000Z</t>
+          <t>2024-07-04T09:35:00.000Z</t>
         </is>
       </c>
       <c r="E107" t="inlineStr"/>
@@ -21782,7 +21782,7 @@
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>2024-07-04T08:35:00.000Z</t>
+          <t>2024-07-04T09:35:00.000Z</t>
         </is>
       </c>
       <c r="E108" t="inlineStr"/>
@@ -21981,7 +21981,7 @@
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>2024-07-04T08:35:00.000Z</t>
+          <t>2024-07-04T09:35:00.000Z</t>
         </is>
       </c>
       <c r="E109" t="inlineStr"/>
@@ -22180,7 +22180,7 @@
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>2024-07-04T08:35:00.000Z</t>
+          <t>2024-07-04T09:35:00.000Z</t>
         </is>
       </c>
       <c r="E110" t="inlineStr"/>
@@ -22379,7 +22379,7 @@
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>2024-07-04T08:32:00.000Z</t>
+          <t>2024-07-04T09:35:00.000Z</t>
         </is>
       </c>
       <c r="E111" t="inlineStr"/>
@@ -22578,7 +22578,7 @@
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>2024-07-04T08:32:00.000Z</t>
+          <t>2024-07-04T09:35:00.000Z</t>
         </is>
       </c>
       <c r="E112" t="inlineStr"/>
@@ -22777,7 +22777,7 @@
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>2024-07-04T08:32:00.000Z</t>
+          <t>2024-07-04T09:35:00.000Z</t>
         </is>
       </c>
       <c r="E113" t="inlineStr"/>
@@ -22976,7 +22976,7 @@
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>2024-07-04T08:32:00.000Z</t>
+          <t>2024-07-04T09:35:00.000Z</t>
         </is>
       </c>
       <c r="E114" t="inlineStr"/>
@@ -23175,7 +23175,7 @@
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>2024-07-04T08:32:00.000Z</t>
+          <t>2024-07-04T09:35:00.000Z</t>
         </is>
       </c>
       <c r="E115" t="inlineStr"/>

</xml_diff>

<commit_message>
fix bug hard code in filter_date function
</commit_message>
<xml_diff>
--- a/notion_data/LUY_KE_NGAY_CAN_THO.xlsx
+++ b/notion_data/LUY_KE_NGAY_CAN_THO.xlsx
@@ -688,7 +688,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2024-07-04T09:36:00.000Z</t>
+          <t>2024-07-04T09:47:00.000Z</t>
         </is>
       </c>
       <c r="E2" t="inlineStr"/>
@@ -887,7 +887,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2024-07-04T09:36:00.000Z</t>
+          <t>2024-07-04T09:47:00.000Z</t>
         </is>
       </c>
       <c r="E3" t="inlineStr"/>
@@ -1086,7 +1086,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>2024-07-04T09:36:00.000Z</t>
+          <t>2024-07-04T09:47:00.000Z</t>
         </is>
       </c>
       <c r="E4" t="inlineStr"/>
@@ -1285,7 +1285,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2024-07-04T09:36:00.000Z</t>
+          <t>2024-07-04T09:47:00.000Z</t>
         </is>
       </c>
       <c r="E5" t="inlineStr"/>
@@ -1484,7 +1484,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2024-07-04T09:36:00.000Z</t>
+          <t>2024-07-04T09:47:00.000Z</t>
         </is>
       </c>
       <c r="E6" t="inlineStr"/>
@@ -1683,7 +1683,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>2024-07-04T09:36:00.000Z</t>
+          <t>2024-07-04T09:47:00.000Z</t>
         </is>
       </c>
       <c r="E7" t="inlineStr"/>
@@ -1882,7 +1882,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>2024-07-04T09:36:00.000Z</t>
+          <t>2024-07-04T09:47:00.000Z</t>
         </is>
       </c>
       <c r="E8" t="inlineStr"/>
@@ -2081,7 +2081,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>2024-07-04T09:36:00.000Z</t>
+          <t>2024-07-04T09:47:00.000Z</t>
         </is>
       </c>
       <c r="E9" t="inlineStr"/>
@@ -2280,7 +2280,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>2024-07-04T09:36:00.000Z</t>
+          <t>2024-07-04T09:47:00.000Z</t>
         </is>
       </c>
       <c r="E10" t="inlineStr"/>
@@ -2479,7 +2479,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>2024-07-04T09:36:00.000Z</t>
+          <t>2024-07-04T09:47:00.000Z</t>
         </is>
       </c>
       <c r="E11" t="inlineStr"/>
@@ -2678,7 +2678,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>2024-07-04T09:36:00.000Z</t>
+          <t>2024-07-04T09:47:00.000Z</t>
         </is>
       </c>
       <c r="E12" t="inlineStr"/>
@@ -2877,7 +2877,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>2024-07-04T09:36:00.000Z</t>
+          <t>2024-07-04T09:47:00.000Z</t>
         </is>
       </c>
       <c r="E13" t="inlineStr"/>
@@ -3076,7 +3076,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>2024-07-04T09:33:00.000Z</t>
+          <t>2024-07-04T09:47:00.000Z</t>
         </is>
       </c>
       <c r="E14" t="inlineStr"/>
@@ -3275,7 +3275,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>2024-07-04T09:33:00.000Z</t>
+          <t>2024-07-04T09:47:00.000Z</t>
         </is>
       </c>
       <c r="E15" t="inlineStr"/>
@@ -3474,7 +3474,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>2024-07-04T09:33:00.000Z</t>
+          <t>2024-07-04T09:47:00.000Z</t>
         </is>
       </c>
       <c r="E16" t="inlineStr"/>
@@ -3673,7 +3673,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>2024-07-04T09:33:00.000Z</t>
+          <t>2024-07-04T09:47:00.000Z</t>
         </is>
       </c>
       <c r="E17" t="inlineStr"/>
@@ -3872,7 +3872,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>2024-07-04T09:33:00.000Z</t>
+          <t>2024-07-04T09:47:00.000Z</t>
         </is>
       </c>
       <c r="E18" t="inlineStr"/>
@@ -4071,7 +4071,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>2024-07-04T09:33:00.000Z</t>
+          <t>2024-07-04T09:47:00.000Z</t>
         </is>
       </c>
       <c r="E19" t="inlineStr"/>
@@ -4270,7 +4270,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>2024-07-04T09:33:00.000Z</t>
+          <t>2024-07-04T09:48:00.000Z</t>
         </is>
       </c>
       <c r="E20" t="inlineStr"/>
@@ -4469,7 +4469,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>2024-07-04T09:33:00.000Z</t>
+          <t>2024-07-04T09:48:00.000Z</t>
         </is>
       </c>
       <c r="E21" t="inlineStr"/>
@@ -4668,7 +4668,7 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>2024-07-04T09:33:00.000Z</t>
+          <t>2024-07-04T09:48:00.000Z</t>
         </is>
       </c>
       <c r="E22" t="inlineStr"/>
@@ -4867,7 +4867,7 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>2024-07-04T09:33:00.000Z</t>
+          <t>2024-07-04T09:48:00.000Z</t>
         </is>
       </c>
       <c r="E23" t="inlineStr"/>
@@ -5066,7 +5066,7 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>2024-07-04T09:33:00.000Z</t>
+          <t>2024-07-04T09:48:00.000Z</t>
         </is>
       </c>
       <c r="E24" t="inlineStr"/>
@@ -5265,7 +5265,7 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>2024-07-04T09:33:00.000Z</t>
+          <t>2024-07-04T09:48:00.000Z</t>
         </is>
       </c>
       <c r="E25" t="inlineStr"/>
@@ -5464,7 +5464,7 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>2024-07-04T09:33:00.000Z</t>
+          <t>2024-07-04T09:48:00.000Z</t>
         </is>
       </c>
       <c r="E26" t="inlineStr"/>
@@ -5663,7 +5663,7 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>2024-07-04T09:33:00.000Z</t>
+          <t>2024-07-04T09:48:00.000Z</t>
         </is>
       </c>
       <c r="E27" t="inlineStr"/>
@@ -5862,7 +5862,7 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>2024-07-04T09:33:00.000Z</t>
+          <t>2024-07-04T09:48:00.000Z</t>
         </is>
       </c>
       <c r="E28" t="inlineStr"/>
@@ -6061,7 +6061,7 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>2024-07-04T09:33:00.000Z</t>
+          <t>2024-07-04T09:48:00.000Z</t>
         </is>
       </c>
       <c r="E29" t="inlineStr"/>
@@ -6260,7 +6260,7 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>2024-07-04T09:33:00.000Z</t>
+          <t>2024-07-04T09:48:00.000Z</t>
         </is>
       </c>
       <c r="E30" t="inlineStr"/>
@@ -6459,7 +6459,7 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>2024-07-04T09:34:00.000Z</t>
+          <t>2024-07-04T09:48:00.000Z</t>
         </is>
       </c>
       <c r="E31" t="inlineStr"/>
@@ -6658,7 +6658,7 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>2024-07-04T09:34:00.000Z</t>
+          <t>2024-07-04T09:48:00.000Z</t>
         </is>
       </c>
       <c r="E32" t="inlineStr"/>
@@ -6857,7 +6857,7 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>2024-07-04T09:34:00.000Z</t>
+          <t>2024-07-04T09:48:00.000Z</t>
         </is>
       </c>
       <c r="E33" t="inlineStr"/>
@@ -7056,7 +7056,7 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>2024-07-04T09:34:00.000Z</t>
+          <t>2024-07-04T09:48:00.000Z</t>
         </is>
       </c>
       <c r="E34" t="inlineStr"/>
@@ -7255,7 +7255,7 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>2024-07-04T09:34:00.000Z</t>
+          <t>2024-07-04T09:48:00.000Z</t>
         </is>
       </c>
       <c r="E35" t="inlineStr"/>
@@ -7454,7 +7454,7 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>2024-07-04T09:34:00.000Z</t>
+          <t>2024-07-04T09:48:00.000Z</t>
         </is>
       </c>
       <c r="E36" t="inlineStr"/>
@@ -7653,7 +7653,7 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>2024-07-04T09:34:00.000Z</t>
+          <t>2024-07-04T09:48:00.000Z</t>
         </is>
       </c>
       <c r="E37" t="inlineStr"/>
@@ -7852,7 +7852,7 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>2024-07-04T09:34:00.000Z</t>
+          <t>2024-07-04T09:48:00.000Z</t>
         </is>
       </c>
       <c r="E38" t="inlineStr"/>
@@ -8051,7 +8051,7 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>2024-07-04T09:34:00.000Z</t>
+          <t>2024-07-04T09:48:00.000Z</t>
         </is>
       </c>
       <c r="E39" t="inlineStr"/>
@@ -8250,7 +8250,7 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>2024-07-04T09:34:00.000Z</t>
+          <t>2024-07-04T09:48:00.000Z</t>
         </is>
       </c>
       <c r="E40" t="inlineStr"/>
@@ -8449,7 +8449,7 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>2024-07-04T09:34:00.000Z</t>
+          <t>2024-07-04T09:47:00.000Z</t>
         </is>
       </c>
       <c r="E41" t="inlineStr"/>
@@ -8648,7 +8648,7 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>2024-07-04T09:34:00.000Z</t>
+          <t>2024-07-04T09:47:00.000Z</t>
         </is>
       </c>
       <c r="E42" t="inlineStr"/>
@@ -8847,7 +8847,7 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>2024-07-04T09:34:00.000Z</t>
+          <t>2024-07-04T09:47:00.000Z</t>
         </is>
       </c>
       <c r="E43" t="inlineStr"/>
@@ -9046,7 +9046,7 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>2024-07-04T09:34:00.000Z</t>
+          <t>2024-07-04T09:47:00.000Z</t>
         </is>
       </c>
       <c r="E44" t="inlineStr"/>
@@ -9245,7 +9245,7 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>2024-07-04T09:34:00.000Z</t>
+          <t>2024-07-04T09:47:00.000Z</t>
         </is>
       </c>
       <c r="E45" t="inlineStr"/>
@@ -9444,7 +9444,7 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>2024-07-04T09:34:00.000Z</t>
+          <t>2024-07-04T09:47:00.000Z</t>
         </is>
       </c>
       <c r="E46" t="inlineStr"/>
@@ -9643,7 +9643,7 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>2024-07-04T09:34:00.000Z</t>
+          <t>2024-07-04T09:47:00.000Z</t>
         </is>
       </c>
       <c r="E47" t="inlineStr"/>
@@ -9842,7 +9842,7 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>2024-07-04T09:34:00.000Z</t>
+          <t>2024-07-04T09:47:00.000Z</t>
         </is>
       </c>
       <c r="E48" t="inlineStr"/>
@@ -10041,7 +10041,7 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>2024-07-04T09:34:00.000Z</t>
+          <t>2024-07-04T09:47:00.000Z</t>
         </is>
       </c>
       <c r="E49" t="inlineStr"/>
@@ -10240,7 +10240,7 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>2024-07-04T09:34:00.000Z</t>
+          <t>2024-07-04T09:47:00.000Z</t>
         </is>
       </c>
       <c r="E50" t="inlineStr"/>
@@ -10439,7 +10439,7 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>2024-07-04T09:34:00.000Z</t>
+          <t>2024-07-04T09:48:00.000Z</t>
         </is>
       </c>
       <c r="E51" t="inlineStr"/>
@@ -10638,7 +10638,7 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>2024-07-04T09:34:00.000Z</t>
+          <t>2024-07-04T09:48:00.000Z</t>
         </is>
       </c>
       <c r="E52" t="inlineStr"/>
@@ -10837,7 +10837,7 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>2024-07-04T09:34:00.000Z</t>
+          <t>2024-07-04T09:48:00.000Z</t>
         </is>
       </c>
       <c r="E53" t="inlineStr"/>
@@ -11036,7 +11036,7 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>2024-07-04T09:34:00.000Z</t>
+          <t>2024-07-04T09:48:00.000Z</t>
         </is>
       </c>
       <c r="E54" t="inlineStr"/>
@@ -11235,7 +11235,7 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>2024-07-04T09:34:00.000Z</t>
+          <t>2024-07-04T09:48:00.000Z</t>
         </is>
       </c>
       <c r="E55" t="inlineStr"/>
@@ -11434,7 +11434,7 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>2024-07-04T09:34:00.000Z</t>
+          <t>2024-07-04T09:48:00.000Z</t>
         </is>
       </c>
       <c r="E56" t="inlineStr"/>
@@ -11633,7 +11633,7 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>2024-07-04T09:34:00.000Z</t>
+          <t>2024-07-04T09:48:00.000Z</t>
         </is>
       </c>
       <c r="E57" t="inlineStr"/>
@@ -11832,7 +11832,7 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>2024-07-04T09:34:00.000Z</t>
+          <t>2024-07-04T09:48:00.000Z</t>
         </is>
       </c>
       <c r="E58" t="inlineStr"/>
@@ -12031,7 +12031,7 @@
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>2024-07-04T09:34:00.000Z</t>
+          <t>2024-07-04T09:48:00.000Z</t>
         </is>
       </c>
       <c r="E59" t="inlineStr"/>
@@ -12230,7 +12230,7 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>2024-07-04T09:34:00.000Z</t>
+          <t>2024-07-04T09:48:00.000Z</t>
         </is>
       </c>
       <c r="E60" t="inlineStr"/>
@@ -12429,7 +12429,7 @@
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>2024-07-04T09:34:00.000Z</t>
+          <t>2024-07-04T09:48:00.000Z</t>
         </is>
       </c>
       <c r="E61" t="inlineStr"/>
@@ -12628,7 +12628,7 @@
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>2024-07-04T09:34:00.000Z</t>
+          <t>2024-07-04T09:48:00.000Z</t>
         </is>
       </c>
       <c r="E62" t="inlineStr"/>
@@ -12827,7 +12827,7 @@
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>2024-07-04T09:34:00.000Z</t>
+          <t>2024-07-04T09:48:00.000Z</t>
         </is>
       </c>
       <c r="E63" t="inlineStr"/>
@@ -13026,7 +13026,7 @@
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>2024-07-04T09:34:00.000Z</t>
+          <t>2024-07-04T09:48:00.000Z</t>
         </is>
       </c>
       <c r="E64" t="inlineStr"/>
@@ -13225,7 +13225,7 @@
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>2024-07-04T09:34:00.000Z</t>
+          <t>2024-07-04T09:48:00.000Z</t>
         </is>
       </c>
       <c r="E65" t="inlineStr"/>
@@ -13424,7 +13424,7 @@
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>2024-07-04T09:34:00.000Z</t>
+          <t>2024-07-04T09:48:00.000Z</t>
         </is>
       </c>
       <c r="E66" t="inlineStr"/>
@@ -13623,7 +13623,7 @@
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>2024-07-04T09:34:00.000Z</t>
+          <t>2024-07-04T09:48:00.000Z</t>
         </is>
       </c>
       <c r="E67" t="inlineStr"/>
@@ -13822,7 +13822,7 @@
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>2024-07-04T09:34:00.000Z</t>
+          <t>2024-07-04T09:48:00.000Z</t>
         </is>
       </c>
       <c r="E68" t="inlineStr"/>
@@ -14021,7 +14021,7 @@
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>2024-07-04T09:34:00.000Z</t>
+          <t>2024-07-04T09:48:00.000Z</t>
         </is>
       </c>
       <c r="E69" t="inlineStr"/>
@@ -14220,7 +14220,7 @@
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>2024-07-04T09:34:00.000Z</t>
+          <t>2024-07-04T09:48:00.000Z</t>
         </is>
       </c>
       <c r="E70" t="inlineStr"/>
@@ -14419,7 +14419,7 @@
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>2024-07-04T09:34:00.000Z</t>
+          <t>2024-07-04T09:48:00.000Z</t>
         </is>
       </c>
       <c r="E71" t="inlineStr"/>
@@ -14618,7 +14618,7 @@
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>2024-07-04T09:34:00.000Z</t>
+          <t>2024-07-04T09:48:00.000Z</t>
         </is>
       </c>
       <c r="E72" t="inlineStr"/>
@@ -14817,7 +14817,7 @@
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>2024-07-04T09:34:00.000Z</t>
+          <t>2024-07-04T09:48:00.000Z</t>
         </is>
       </c>
       <c r="E73" t="inlineStr"/>
@@ -15016,7 +15016,7 @@
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>2024-07-04T09:34:00.000Z</t>
+          <t>2024-07-04T09:48:00.000Z</t>
         </is>
       </c>
       <c r="E74" t="inlineStr"/>
@@ -15215,7 +15215,7 @@
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>2024-07-04T09:34:00.000Z</t>
+          <t>2024-07-04T09:48:00.000Z</t>
         </is>
       </c>
       <c r="E75" t="inlineStr"/>
@@ -15414,7 +15414,7 @@
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>2024-07-04T09:34:00.000Z</t>
+          <t>2024-07-04T09:48:00.000Z</t>
         </is>
       </c>
       <c r="E76" t="inlineStr"/>
@@ -15613,7 +15613,7 @@
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>2024-07-04T09:35:00.000Z</t>
+          <t>2024-07-04T09:48:00.000Z</t>
         </is>
       </c>
       <c r="E77" t="inlineStr"/>
@@ -15812,7 +15812,7 @@
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>2024-07-04T09:35:00.000Z</t>
+          <t>2024-07-04T09:48:00.000Z</t>
         </is>
       </c>
       <c r="E78" t="inlineStr"/>
@@ -16011,7 +16011,7 @@
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>2024-07-04T09:35:00.000Z</t>
+          <t>2024-07-04T09:48:00.000Z</t>
         </is>
       </c>
       <c r="E79" t="inlineStr"/>
@@ -16210,7 +16210,7 @@
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>2024-07-04T09:35:00.000Z</t>
+          <t>2024-07-04T09:48:00.000Z</t>
         </is>
       </c>
       <c r="E80" t="inlineStr"/>
@@ -16409,7 +16409,7 @@
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>2024-07-04T09:35:00.000Z</t>
+          <t>2024-07-04T09:48:00.000Z</t>
         </is>
       </c>
       <c r="E81" t="inlineStr"/>
@@ -16608,7 +16608,7 @@
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>2024-07-04T09:35:00.000Z</t>
+          <t>2024-07-04T09:48:00.000Z</t>
         </is>
       </c>
       <c r="E82" t="inlineStr"/>
@@ -16807,7 +16807,7 @@
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>2024-07-04T09:35:00.000Z</t>
+          <t>2024-07-04T09:48:00.000Z</t>
         </is>
       </c>
       <c r="E83" t="inlineStr"/>
@@ -17006,7 +17006,7 @@
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>2024-07-04T09:35:00.000Z</t>
+          <t>2024-07-04T09:48:00.000Z</t>
         </is>
       </c>
       <c r="E84" t="inlineStr"/>
@@ -17205,7 +17205,7 @@
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>2024-07-04T09:35:00.000Z</t>
+          <t>2024-07-04T09:48:00.000Z</t>
         </is>
       </c>
       <c r="E85" t="inlineStr"/>
@@ -17404,7 +17404,7 @@
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>2024-07-04T09:35:00.000Z</t>
+          <t>2024-07-04T09:48:00.000Z</t>
         </is>
       </c>
       <c r="E86" t="inlineStr"/>
@@ -17603,7 +17603,7 @@
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>2024-07-04T09:35:00.000Z</t>
+          <t>2024-07-04T09:48:00.000Z</t>
         </is>
       </c>
       <c r="E87" t="inlineStr"/>
@@ -17802,7 +17802,7 @@
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>2024-07-04T09:35:00.000Z</t>
+          <t>2024-07-04T09:44:00.000Z</t>
         </is>
       </c>
       <c r="E88" t="inlineStr"/>
@@ -18001,7 +18001,7 @@
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>2024-07-04T09:35:00.000Z</t>
+          <t>2024-07-04T09:44:00.000Z</t>
         </is>
       </c>
       <c r="E89" t="inlineStr"/>
@@ -18200,7 +18200,7 @@
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>2024-07-04T09:35:00.000Z</t>
+          <t>2024-07-04T09:44:00.000Z</t>
         </is>
       </c>
       <c r="E90" t="inlineStr"/>
@@ -18399,7 +18399,7 @@
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>2024-07-04T09:35:00.000Z</t>
+          <t>2024-07-04T09:44:00.000Z</t>
         </is>
       </c>
       <c r="E91" t="inlineStr"/>
@@ -18598,7 +18598,7 @@
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>2024-07-04T09:35:00.000Z</t>
+          <t>2024-07-04T09:44:00.000Z</t>
         </is>
       </c>
       <c r="E92" t="inlineStr"/>
@@ -18797,7 +18797,7 @@
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>2024-07-04T09:35:00.000Z</t>
+          <t>2024-07-04T09:44:00.000Z</t>
         </is>
       </c>
       <c r="E93" t="inlineStr"/>
@@ -18996,7 +18996,7 @@
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>2024-07-04T09:35:00.000Z</t>
+          <t>2024-07-04T09:44:00.000Z</t>
         </is>
       </c>
       <c r="E94" t="inlineStr"/>
@@ -19195,7 +19195,7 @@
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>2024-07-04T09:35:00.000Z</t>
+          <t>2024-07-04T09:44:00.000Z</t>
         </is>
       </c>
       <c r="E95" t="inlineStr"/>
@@ -19394,7 +19394,7 @@
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>2024-07-04T09:35:00.000Z</t>
+          <t>2024-07-04T09:44:00.000Z</t>
         </is>
       </c>
       <c r="E96" t="inlineStr"/>
@@ -19593,7 +19593,7 @@
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>2024-07-04T09:35:00.000Z</t>
+          <t>2024-07-04T09:45:00.000Z</t>
         </is>
       </c>
       <c r="E97" t="inlineStr"/>
@@ -19792,7 +19792,7 @@
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>2024-07-04T09:35:00.000Z</t>
+          <t>2024-07-04T09:45:00.000Z</t>
         </is>
       </c>
       <c r="E98" t="inlineStr"/>
@@ -19991,7 +19991,7 @@
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>2024-07-04T09:35:00.000Z</t>
+          <t>2024-07-04T09:45:00.000Z</t>
         </is>
       </c>
       <c r="E99" t="inlineStr"/>
@@ -20190,7 +20190,7 @@
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>2024-07-04T09:35:00.000Z</t>
+          <t>2024-07-04T09:45:00.000Z</t>
         </is>
       </c>
       <c r="E100" t="inlineStr"/>
@@ -20389,7 +20389,7 @@
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>2024-07-04T09:35:00.000Z</t>
+          <t>2024-07-04T09:45:00.000Z</t>
         </is>
       </c>
       <c r="E101" t="inlineStr"/>
@@ -20588,7 +20588,7 @@
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>2024-07-04T09:35:00.000Z</t>
+          <t>2024-07-04T09:45:00.000Z</t>
         </is>
       </c>
       <c r="E102" t="inlineStr"/>
@@ -20787,7 +20787,7 @@
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>2024-07-04T09:35:00.000Z</t>
+          <t>2024-07-04T09:45:00.000Z</t>
         </is>
       </c>
       <c r="E103" t="inlineStr"/>
@@ -20986,7 +20986,7 @@
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>2024-07-04T09:35:00.000Z</t>
+          <t>2024-07-04T09:45:00.000Z</t>
         </is>
       </c>
       <c r="E104" t="inlineStr"/>
@@ -21185,7 +21185,7 @@
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>2024-07-04T09:35:00.000Z</t>
+          <t>2024-07-04T09:45:00.000Z</t>
         </is>
       </c>
       <c r="E105" t="inlineStr"/>
@@ -21384,7 +21384,7 @@
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>2024-07-04T09:35:00.000Z</t>
+          <t>2024-07-04T09:45:00.000Z</t>
         </is>
       </c>
       <c r="E106" t="inlineStr"/>
@@ -21583,7 +21583,7 @@
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>2024-07-04T09:35:00.000Z</t>
+          <t>2024-07-04T09:45:00.000Z</t>
         </is>
       </c>
       <c r="E107" t="inlineStr"/>
@@ -21782,7 +21782,7 @@
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>2024-07-04T09:35:00.000Z</t>
+          <t>2024-07-04T09:45:00.000Z</t>
         </is>
       </c>
       <c r="E108" t="inlineStr"/>
@@ -21981,7 +21981,7 @@
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>2024-07-04T09:35:00.000Z</t>
+          <t>2024-07-04T09:45:00.000Z</t>
         </is>
       </c>
       <c r="E109" t="inlineStr"/>
@@ -22180,7 +22180,7 @@
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>2024-07-04T09:35:00.000Z</t>
+          <t>2024-07-04T09:45:00.000Z</t>
         </is>
       </c>
       <c r="E110" t="inlineStr"/>
@@ -22379,7 +22379,7 @@
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>2024-07-04T09:35:00.000Z</t>
+          <t>2024-07-04T09:45:00.000Z</t>
         </is>
       </c>
       <c r="E111" t="inlineStr"/>
@@ -22578,7 +22578,7 @@
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>2024-07-04T09:35:00.000Z</t>
+          <t>2024-07-04T09:45:00.000Z</t>
         </is>
       </c>
       <c r="E112" t="inlineStr"/>
@@ -22777,7 +22777,7 @@
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>2024-07-04T09:35:00.000Z</t>
+          <t>2024-07-04T09:45:00.000Z</t>
         </is>
       </c>
       <c r="E113" t="inlineStr"/>
@@ -22976,7 +22976,7 @@
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>2024-07-04T09:35:00.000Z</t>
+          <t>2024-07-04T09:45:00.000Z</t>
         </is>
       </c>
       <c r="E114" t="inlineStr"/>
@@ -23175,7 +23175,7 @@
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>2024-07-04T09:35:00.000Z</t>
+          <t>2024-07-04T09:45:00.000Z</t>
         </is>
       </c>
       <c r="E115" t="inlineStr"/>

</xml_diff>